<commit_message>
Change year using for index to 2013 so aligns with heating demand data
</commit_message>
<xml_diff>
--- a/docs/solar_year_on_year_variability.xlsx
+++ b/docs/solar_year_on_year_variability.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniewillis/Code/heat-pump-and_solar-savings/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB6DF30-76F8-A140-A203-E0CEAE2FC61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D03623-FD93-C145-BFB9-E366B4C53990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="760" windowWidth="10000" windowHeight="15700" activeTab="1" xr2:uid="{02E8AA48-D886-A043-8C2E-364EA90E1972}"/>
+    <workbookView xWindow="1500" yWindow="760" windowWidth="10880" windowHeight="15700" activeTab="1" xr2:uid="{02E8AA48-D886-A043-8C2E-364EA90E1972}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="variability by region" sheetId="1" r:id="rId1"/>
+    <sheet name="typical years" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Year on year variability tests</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Year to year standard deviation</t>
   </si>
   <si>
-    <t>Test params</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -82,13 +79,25 @@
   </si>
   <si>
     <t>Average:</t>
+  </si>
+  <si>
+    <t>Test params with API</t>
+  </si>
+  <si>
+    <t>4kW of capacity</t>
+  </si>
+  <si>
+    <t>3kW of capacity</t>
+  </si>
+  <si>
+    <t>Initially used 2020, but now using 2013 as heating demand profiles are for 2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,12 +129,6 @@
     </font>
     <font>
       <sz val="9.8000000000000007"/>
-      <color rgb="FFAA4926"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
       <color rgb="FFCC7832"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
@@ -133,6 +136,22 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -156,10 +175,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -167,9 +187,11 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
@@ -595,7 +617,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -616,7 +638,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -695,34 +717,37 @@
       <c r="D12" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{2604B34C-FAC4-C840-9C76-3539425644AD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38ADF75E-7891-334E-8FEC-7BB25B6C42CE}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="7" t="s">
-        <v>8</v>
+      <c r="A1" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21">
-      <c r="A2" s="7"/>
+      <c r="A2" s="6"/>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>51.680999999999997</v>
@@ -730,7 +755,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>-3.7240000000000002</v>
@@ -738,23 +763,25 @@
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="F5" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="C6" s="5"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -772,6 +799,9 @@
       <c r="C9">
         <v>3028</v>
       </c>
+      <c r="D9">
+        <v>2271.1216800000002</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10">
@@ -783,18 +813,32 @@
     </row>
     <row r="11" spans="1:6">
       <c r="B11">
+        <v>2013</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11">
+        <v>2239.14921</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12">
         <v>2012</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>2836.5539999999901</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="3">
+    <row r="15" spans="1:6">
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3">
         <v>3000.66</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>